<commit_message>
Adapt Micronaut v4.5.0. Minimum required jvm version is now 17. javax package is replaced by jakarta package, but SQL related.
</commit_message>
<xml_diff>
--- a/blanco-meta/rest/SampleArrayPayloadTest.xlsx
+++ b/blanco-meta/rest/SampleArrayPayloadTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/rest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63D7F8D-A503-EE41-A267-A26E35628F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24099E8-F55D-6E47-A467-7CB7C68531F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="641" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="641" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -18,11 +18,13 @@
     <sheet name="get_output" sheetId="32" r:id="rId3"/>
     <sheet name="post_input" sheetId="29" r:id="rId4"/>
     <sheet name="post_output" sheetId="30" r:id="rId5"/>
-    <sheet name="readme" sheetId="17" r:id="rId6"/>
-    <sheet name="config" sheetId="3" r:id="rId7"/>
+    <sheet name="put_input" sheetId="33" r:id="rId6"/>
+    <sheet name="put_output" sheetId="34" r:id="rId7"/>
+    <sheet name="readme" sheetId="17" r:id="rId8"/>
+    <sheet name="config" sheetId="3" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="isImport">config!$E$5:$E$6</definedName>
@@ -37,6 +39,8 @@
     <definedName name="項目型" localSheetId="2">config!#REF!</definedName>
     <definedName name="項目型" localSheetId="3">config!#REF!</definedName>
     <definedName name="項目型" localSheetId="4">config!#REF!</definedName>
+    <definedName name="項目型" localSheetId="5">config!#REF!</definedName>
+    <definedName name="項目型" localSheetId="6">config!#REF!</definedName>
     <definedName name="項目型">config!#REF!</definedName>
     <definedName name="必須">config!$C$5:$C$6</definedName>
     <definedName name="必須フラグ">config!$B$5:$B$7</definedName>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="217">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2183,25 +2187,9 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>javax.validation.constraints.Size</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>@field:Size(max = 50)
 @field:NotBlank
 @field:Pattern(regexp = "^((?=.*[a-z])(?=.*[A-Z])(?=.*[0-9])|(?=.*[a-z])(?=.*[A-Z])(?=.*[@%\\+\\/\\\'!#\\$\\^\\?:\\.\\(\\)\\{\\}\\[\\]~\\-_])|(?=.*[a-z])(?=.*[0-9])(?=.*[@%\\+\\/\\\'!#\\$\\^\\?:\\.\\(\\)\\{\\}\\[\\]~\\-_])|(?=.*[A-Z])(?=.*[0-9])(?=.*[@%\\+\\/\\\'!#\\$\\^\\?:\\.\\(\\)\\{\\}\\[\\]~\\-_]))[a-zA-Z0-9@%\\+\\/\\\'!#\\$\\^\\?:\\.\\(\\)\\{\\}\\[\\]~\\-_]{8,20}$")</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>javax.validation.constraints.NotBlank</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>javax.validation.constraints.Pattern</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>javax.validation.Valid</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -2398,6 +2386,45 @@
   <si>
     <t>sample_array</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>jakarta.validation.constraints.Size</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>jakarta.validation.constraints.NotBlank</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>jakarta.validation.constraints.Pattern</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>jakarta.validation.Valid</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>電文がOption</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>/* ペイロード電文が省略可能 */</t>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PUT</t>
   </si>
 </sst>
 </file>
@@ -4397,7 +4424,7 @@
       <c r="B6" s="150"/>
       <c r="C6" s="151"/>
       <c r="D6" s="146" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E6" s="146"/>
     </row>
@@ -4408,7 +4435,7 @@
       <c r="B7" s="152"/>
       <c r="C7" s="152"/>
       <c r="D7" s="147" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E7" s="148"/>
     </row>
@@ -4419,7 +4446,7 @@
       <c r="B8" s="145"/>
       <c r="C8" s="145"/>
       <c r="D8" s="146" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E8" s="146"/>
     </row>
@@ -4439,7 +4466,7 @@
       <c r="B10" s="145"/>
       <c r="C10" s="145"/>
       <c r="D10" s="146" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E10" s="146"/>
     </row>
@@ -4450,7 +4477,7 @@
       <c r="B11" s="145"/>
       <c r="C11" s="145"/>
       <c r="D11" s="146" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E11" s="146"/>
     </row>
@@ -4501,7 +4528,7 @@
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
       <c r="D15" s="135" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E15" s="136"/>
       <c r="F15" s="1" t="s">
@@ -4515,7 +4542,7 @@
       <c r="B16" s="134"/>
       <c r="C16" s="134"/>
       <c r="D16" s="135" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E16" s="136"/>
       <c r="F16" s="1" t="s">
@@ -4602,7 +4629,7 @@
       <c r="B23" s="90"/>
       <c r="C23" s="76"/>
       <c r="D23" s="73" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E23" s="74"/>
       <c r="F23" s="74"/>
@@ -4834,7 +4861,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="162" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C40" s="162"/>
       <c r="D40" s="162"/>
@@ -5080,8 +5107,8 @@
   </sheetPr>
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5160,7 +5187,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="42" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D7" s="103"/>
       <c r="S7"/>
@@ -5181,7 +5208,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="97" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -5215,7 +5242,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="146" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D13" s="146"/>
     </row>
@@ -5225,7 +5252,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="146" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D14" s="146"/>
       <c r="I14"/>
@@ -5492,7 +5519,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="162" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="C28" s="162"/>
       <c r="D28" s="162"/>
@@ -5513,7 +5540,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="162" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="C29" s="162"/>
       <c r="D29" s="162"/>
@@ -5534,7 +5561,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="162" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="C30" s="162"/>
       <c r="D30" s="162"/>
@@ -5801,10 +5828,10 @@
         <v>171</v>
       </c>
       <c r="M42" s="197" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="N42" s="197" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O42" s="188" t="s">
         <v>148</v>
@@ -5862,10 +5889,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>92</v>
@@ -5881,14 +5908,14 @@
       <c r="I44" s="120"/>
       <c r="J44" s="120"/>
       <c r="K44" s="127" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="L44" s="120" t="s">
         <v>158</v>
       </c>
       <c r="M44" s="120"/>
       <c r="N44" s="120" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="O44" s="23"/>
       <c r="P44" s="19"/>
@@ -5925,7 +5952,7 @@
       <c r="I45" s="121"/>
       <c r="J45" s="121"/>
       <c r="K45" s="128" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L45" s="121" t="s">
         <v>158</v>
@@ -6331,8 +6358,8 @@
   </sheetPr>
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:D43"/>
+    <sheetView zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -6411,7 +6438,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="42" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D7" s="31"/>
       <c r="Q7"/>
@@ -6432,7 +6459,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D9" s="72"/>
     </row>
@@ -6442,7 +6469,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="146" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D10" s="146"/>
     </row>
@@ -6452,7 +6479,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="146" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D11" s="146"/>
     </row>
@@ -6475,7 +6502,7 @@
       </c>
       <c r="B13" s="98"/>
       <c r="C13" s="135" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D13" s="136"/>
     </row>
@@ -6504,14 +6531,14 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="99" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B15" s="100"/>
       <c r="C15" s="77" t="s">
         <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -6679,7 +6706,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="162" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="C25" s="162"/>
       <c r="D25" s="162"/>
@@ -6703,7 +6730,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="162" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="C26" s="162"/>
       <c r="D26" s="162"/>
@@ -6727,7 +6754,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="163" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="C27" s="163"/>
       <c r="D27" s="163"/>
@@ -6751,7 +6778,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="162" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="C28" s="162"/>
       <c r="D28" s="162"/>
@@ -6772,7 +6799,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="162" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C29" s="162"/>
       <c r="D29" s="162"/>
@@ -7072,10 +7099,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>92</v>
@@ -7102,13 +7129,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="112" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D43" s="113" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E43" s="54"/>
       <c r="F43" s="54"/>
@@ -7368,8 +7395,8 @@
   </sheetPr>
   <dimension ref="A1:V96"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7448,7 +7475,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="42" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D7" s="103"/>
       <c r="S7"/>
@@ -7503,7 +7530,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="146" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D13" s="146"/>
     </row>
@@ -7513,7 +7540,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="146" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D14" s="146"/>
       <c r="I14"/>
@@ -7608,14 +7635,14 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="99" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B19" s="100"/>
       <c r="C19" s="77" t="s">
         <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
@@ -7800,7 +7827,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="162" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="C29" s="162"/>
       <c r="D29" s="162"/>
@@ -7821,7 +7848,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="162" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="C30" s="162"/>
       <c r="D30" s="162"/>
@@ -7842,7 +7869,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="162" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="C31" s="162"/>
       <c r="D31" s="162"/>
@@ -8109,10 +8136,10 @@
         <v>171</v>
       </c>
       <c r="M43" s="197" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="N43" s="197" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O43" s="188" t="s">
         <v>148</v>
@@ -8170,10 +8197,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>92</v>
@@ -8189,14 +8216,14 @@
       <c r="I45" s="120"/>
       <c r="J45" s="120"/>
       <c r="K45" s="127" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="L45" s="120" t="s">
         <v>158</v>
       </c>
       <c r="M45" s="120"/>
       <c r="N45" s="120" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="O45" s="23"/>
       <c r="P45" s="19"/>
@@ -8233,7 +8260,7 @@
       <c r="I46" s="121"/>
       <c r="J46" s="121"/>
       <c r="K46" s="128" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L46" s="121" t="s">
         <v>158</v>
@@ -8638,7 +8665,7 @@
   <dimension ref="A1:T65"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="A32" sqref="A32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8717,7 +8744,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="42" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D7" s="31"/>
       <c r="Q7"/>
@@ -8748,7 +8775,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="146" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D10" s="146"/>
     </row>
@@ -8758,7 +8785,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="146" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D11" s="146"/>
     </row>
@@ -8808,14 +8835,14 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="99" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B15" s="100"/>
       <c r="C15" s="77" t="s">
         <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -8983,7 +9010,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="162" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="C25" s="162"/>
       <c r="D25" s="162"/>
@@ -9007,7 +9034,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="162" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="C26" s="162"/>
       <c r="D26" s="162"/>
@@ -9031,7 +9058,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="163" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="C27" s="163"/>
       <c r="D27" s="163"/>
@@ -9055,7 +9082,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="162" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="C28" s="162"/>
       <c r="D28" s="162"/>
@@ -9372,10 +9399,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>92</v>
@@ -9402,13 +9429,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="112" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D43" s="113" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E43" s="54"/>
       <c r="F43" s="54"/>
@@ -9662,6 +9689,2326 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FF9966-C4AB-EE42-97CC-BBAE13567341}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:V97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="20.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" style="1" customWidth="1"/>
+    <col min="12" max="14" width="20.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.83203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="43.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="6.1640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="18.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.33203125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.83203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="8.83203125" style="1"/>
+    <col min="33" max="33" width="9.1640625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="19">
+      <c r="A1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="104" t="str">
+        <f>process!D6&amp;PROPER(C9)&amp;IF(C8="要求電文(C→S)", "Request", "Response")</f>
+        <v>SampleArrayPayloadTestPutRequest</v>
+      </c>
+      <c r="D6" s="105"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="103"/>
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="101"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="97" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="102"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="146" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="146"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="146" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="146"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="98"/>
+      <c r="C15" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="136"/>
+      <c r="E15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="98"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="99" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="100"/>
+      <c r="C17" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="107" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="108"/>
+      <c r="C18" s="77"/>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="99" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="100"/>
+      <c r="C19" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>203</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="99" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="100"/>
+      <c r="C20" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>215</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="6"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="178" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="178"/>
+      <c r="C22" s="178"/>
+      <c r="D22" s="178"/>
+      <c r="E22" s="178"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="178"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="172" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="173"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="174"/>
+      <c r="H23" s="82"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23" s="82"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
+      <c r="S23" s="82"/>
+      <c r="U23" s="88"/>
+      <c r="V23" s="88"/>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" s="93"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="155"/>
+      <c r="H24" s="89"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24" s="89"/>
+      <c r="P24" s="89"/>
+      <c r="Q24" s="89"/>
+      <c r="R24" s="89"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="A25" s="94"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="89"/>
+      <c r="Q25" s="89"/>
+      <c r="R25" s="89"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="95"/>
+      <c r="B26" s="157"/>
+      <c r="C26" s="157"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="157"/>
+      <c r="F26" s="157"/>
+      <c r="G26" s="157"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="82"/>
+      <c r="O26" s="89"/>
+      <c r="P26" s="89"/>
+      <c r="Q26" s="89"/>
+      <c r="R26" s="89"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="C27"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="82"/>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28" s="175" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="176"/>
+      <c r="C28" s="176"/>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="177"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="A29" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="161" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="161"/>
+      <c r="D29" s="161"/>
+      <c r="E29" s="161"/>
+      <c r="F29" s="161"/>
+      <c r="G29" s="161"/>
+      <c r="H29" s="82"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29" s="82"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="82"/>
+      <c r="R29" s="82"/>
+      <c r="S29" s="82"/>
+      <c r="U29" s="88"/>
+      <c r="V29" s="88"/>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30" s="93">
+        <v>1</v>
+      </c>
+      <c r="B30" s="162" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" s="162"/>
+      <c r="D30" s="162"/>
+      <c r="E30" s="162"/>
+      <c r="F30" s="162"/>
+      <c r="G30" s="162"/>
+      <c r="H30" s="89"/>
+      <c r="O30" s="89"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="89"/>
+      <c r="R30" s="89"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" s="93">
+        <v>2</v>
+      </c>
+      <c r="B31" s="162" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="162"/>
+      <c r="D31" s="162"/>
+      <c r="E31" s="162"/>
+      <c r="F31" s="162"/>
+      <c r="G31" s="162"/>
+      <c r="H31" s="89"/>
+      <c r="O31" s="89"/>
+      <c r="P31" s="89"/>
+      <c r="Q31" s="89"/>
+      <c r="R31" s="89"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32" s="93">
+        <v>3</v>
+      </c>
+      <c r="B32" s="162" t="s">
+        <v>212</v>
+      </c>
+      <c r="C32" s="162"/>
+      <c r="D32" s="162"/>
+      <c r="E32" s="162"/>
+      <c r="F32" s="162"/>
+      <c r="G32" s="162"/>
+      <c r="H32" s="89"/>
+      <c r="O32" s="89"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="89"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33" s="94"/>
+      <c r="B33" s="163"/>
+      <c r="C33" s="163"/>
+      <c r="D33" s="163"/>
+      <c r="E33" s="163"/>
+      <c r="F33" s="163"/>
+      <c r="G33" s="163"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="89"/>
+      <c r="P33" s="89"/>
+      <c r="Q33" s="89"/>
+      <c r="R33" s="89"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="A34" s="95"/>
+      <c r="B34" s="164"/>
+      <c r="C34" s="164"/>
+      <c r="D34" s="164"/>
+      <c r="E34" s="164"/>
+      <c r="F34" s="164"/>
+      <c r="G34" s="164"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="89"/>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="89"/>
+      <c r="R34" s="89"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36" s="175" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="176"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="176"/>
+      <c r="E36" s="176"/>
+      <c r="F36" s="176"/>
+      <c r="G36" s="177"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="161" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="161"/>
+      <c r="D37" s="161"/>
+      <c r="E37" s="161"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="161"/>
+      <c r="H37" s="82"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="82"/>
+      <c r="Q37" s="82"/>
+      <c r="R37" s="82"/>
+      <c r="S37" s="82"/>
+      <c r="U37" s="88"/>
+      <c r="V37" s="88"/>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38" s="93"/>
+      <c r="B38" s="155"/>
+      <c r="C38" s="155"/>
+      <c r="D38" s="155"/>
+      <c r="E38" s="155"/>
+      <c r="F38" s="155"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="89"/>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89"/>
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="A39" s="94"/>
+      <c r="B39" s="156"/>
+      <c r="C39" s="156"/>
+      <c r="D39" s="156"/>
+      <c r="E39" s="156"/>
+      <c r="F39" s="156"/>
+      <c r="G39" s="186"/>
+      <c r="H39" s="89"/>
+      <c r="O39" s="89"/>
+      <c r="P39" s="89"/>
+      <c r="Q39" s="89"/>
+      <c r="R39" s="89"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" s="95"/>
+      <c r="B40" s="157"/>
+      <c r="C40" s="157"/>
+      <c r="D40" s="157"/>
+      <c r="E40" s="157"/>
+      <c r="F40" s="157"/>
+      <c r="G40" s="187"/>
+      <c r="H40" s="89"/>
+      <c r="O40" s="89"/>
+      <c r="P40" s="89"/>
+      <c r="Q40" s="89"/>
+      <c r="R40" s="89"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" s="6"/>
+      <c r="I42" s="118"/>
+      <c r="J42" s="118"/>
+      <c r="K42" s="118"/>
+      <c r="L42" s="118"/>
+      <c r="M42" s="118"/>
+      <c r="N42" s="118"/>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="119"/>
+      <c r="J43" s="119"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="119"/>
+      <c r="M43" s="119"/>
+      <c r="N43" s="119"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="5"/>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" s="188" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="188" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="190" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="188" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="191" t="s">
+        <v>129</v>
+      </c>
+      <c r="F44" s="191" t="s">
+        <v>132</v>
+      </c>
+      <c r="G44" s="188" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="I44" s="196" t="s">
+        <v>168</v>
+      </c>
+      <c r="J44" s="196" t="s">
+        <v>169</v>
+      </c>
+      <c r="K44" s="196" t="s">
+        <v>170</v>
+      </c>
+      <c r="L44" s="197" t="s">
+        <v>171</v>
+      </c>
+      <c r="M44" s="197" t="s">
+        <v>194</v>
+      </c>
+      <c r="N44" s="197" t="s">
+        <v>195</v>
+      </c>
+      <c r="O44" s="188" t="s">
+        <v>148</v>
+      </c>
+      <c r="P44" s="194" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q44" s="195"/>
+      <c r="R44" s="194" t="s">
+        <v>17</v>
+      </c>
+      <c r="S44" s="195"/>
+      <c r="T44" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="U44" s="188" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" s="189"/>
+      <c r="B45" s="189"/>
+      <c r="C45" s="189"/>
+      <c r="D45" s="189"/>
+      <c r="E45" s="192"/>
+      <c r="F45" s="193"/>
+      <c r="G45" s="189"/>
+      <c r="H45" s="189"/>
+      <c r="I45" s="196"/>
+      <c r="J45" s="196"/>
+      <c r="K45" s="196"/>
+      <c r="L45" s="198"/>
+      <c r="M45" s="198"/>
+      <c r="N45" s="198"/>
+      <c r="O45" s="199"/>
+      <c r="P45" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q45" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="R45" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="S45" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="T45" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="U45" s="189"/>
+    </row>
+    <row r="46" spans="1:22" ht="45">
+      <c r="A46" s="7">
+        <v>1</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I46" s="120"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="127" t="s">
+        <v>177</v>
+      </c>
+      <c r="L46" s="120" t="s">
+        <v>158</v>
+      </c>
+      <c r="M46" s="120"/>
+      <c r="N46" s="120" t="s">
+        <v>196</v>
+      </c>
+      <c r="O46" s="23"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="28">
+        <v>254</v>
+      </c>
+      <c r="R46" s="22"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+      <c r="U46" s="9"/>
+    </row>
+    <row r="47" spans="1:22" ht="370">
+      <c r="A47" s="10">
+        <f>A46+1</f>
+        <v>2</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="I47" s="121"/>
+      <c r="J47" s="121"/>
+      <c r="K47" s="128" t="s">
+        <v>172</v>
+      </c>
+      <c r="L47" s="121" t="s">
+        <v>158</v>
+      </c>
+      <c r="M47" s="121"/>
+      <c r="N47" s="121"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="28">
+        <v>50</v>
+      </c>
+      <c r="R47" s="19"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="28"/>
+      <c r="U47" s="12"/>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48" s="10"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="121"/>
+      <c r="J48" s="121"/>
+      <c r="K48" s="128"/>
+      <c r="L48" s="121"/>
+      <c r="M48" s="121"/>
+      <c r="N48" s="121"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="28"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="28"/>
+      <c r="T48" s="28"/>
+      <c r="U48" s="12"/>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49" s="14"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="124"/>
+      <c r="J49" s="125"/>
+      <c r="K49" s="125"/>
+      <c r="L49" s="126"/>
+      <c r="M49" s="126"/>
+      <c r="N49" s="126"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="29"/>
+      <c r="T49" s="29"/>
+      <c r="U49" s="16"/>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="I50" s="123"/>
+      <c r="J50" s="123"/>
+      <c r="K50" s="123"/>
+      <c r="L50" s="123"/>
+      <c r="M50" s="123"/>
+      <c r="N50" s="123"/>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="I52" s="123"/>
+      <c r="J52" s="123"/>
+      <c r="K52" s="123"/>
+      <c r="L52" s="123"/>
+      <c r="M52" s="123"/>
+      <c r="N52" s="123"/>
+    </row>
+    <row r="54" spans="1:21">
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
+      <c r="N54" s="123"/>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+      <c r="M60" s="82"/>
+      <c r="N60" s="82"/>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="I61" s="82"/>
+      <c r="J61" s="82"/>
+      <c r="K61" s="82"/>
+      <c r="L61" s="82"/>
+      <c r="M61" s="82"/>
+      <c r="N61" s="82"/>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="I62" s="82"/>
+      <c r="J62" s="82"/>
+      <c r="K62" s="82"/>
+      <c r="L62" s="82"/>
+      <c r="M62" s="82"/>
+      <c r="N62" s="82"/>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="82"/>
+      <c r="L63" s="82"/>
+      <c r="M63" s="82"/>
+      <c r="N63" s="82"/>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="I64" s="82"/>
+      <c r="J64" s="82"/>
+      <c r="K64" s="82"/>
+      <c r="L64" s="82"/>
+      <c r="M64" s="82"/>
+      <c r="N64" s="82"/>
+    </row>
+    <row r="65" spans="9:14">
+      <c r="I65" s="82"/>
+      <c r="J65" s="82"/>
+      <c r="K65" s="82"/>
+      <c r="L65" s="82"/>
+      <c r="M65" s="82"/>
+      <c r="N65" s="82"/>
+    </row>
+    <row r="66" spans="9:14">
+      <c r="I66" s="82"/>
+      <c r="J66" s="82"/>
+      <c r="K66" s="82"/>
+      <c r="L66" s="82"/>
+      <c r="M66" s="82"/>
+      <c r="N66" s="82"/>
+    </row>
+    <row r="67" spans="9:14">
+      <c r="I67" s="82"/>
+      <c r="J67" s="82"/>
+      <c r="K67" s="82"/>
+      <c r="L67" s="82"/>
+      <c r="M67" s="82"/>
+      <c r="N67" s="82"/>
+    </row>
+    <row r="68" spans="9:14">
+      <c r="I68" s="82"/>
+      <c r="J68" s="82"/>
+      <c r="K68" s="82"/>
+      <c r="L68" s="82"/>
+      <c r="M68" s="82"/>
+      <c r="N68" s="82"/>
+    </row>
+    <row r="69" spans="9:14">
+      <c r="I69" s="82"/>
+      <c r="J69" s="82"/>
+      <c r="K69" s="82"/>
+      <c r="L69" s="82"/>
+      <c r="M69" s="82"/>
+      <c r="N69" s="82"/>
+    </row>
+    <row r="71" spans="9:14">
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+    </row>
+    <row r="72" spans="9:14">
+      <c r="I72" s="88"/>
+      <c r="J72" s="88"/>
+      <c r="K72" s="88"/>
+      <c r="L72" s="88"/>
+      <c r="M72" s="88"/>
+      <c r="N72" s="88"/>
+    </row>
+    <row r="73" spans="9:14">
+      <c r="I73" s="88"/>
+      <c r="J73" s="88"/>
+      <c r="K73" s="88"/>
+      <c r="L73" s="88"/>
+      <c r="M73" s="88"/>
+      <c r="N73" s="88"/>
+    </row>
+    <row r="74" spans="9:14">
+      <c r="K74" s="123"/>
+    </row>
+    <row r="75" spans="9:14">
+      <c r="K75" s="123"/>
+    </row>
+    <row r="78" spans="9:14">
+      <c r="I78" s="123"/>
+      <c r="J78" s="123"/>
+      <c r="K78" s="123"/>
+      <c r="L78" s="123"/>
+      <c r="M78" s="123"/>
+      <c r="N78" s="123"/>
+    </row>
+    <row r="80" spans="9:14">
+      <c r="I80" s="123"/>
+      <c r="J80" s="123"/>
+      <c r="K80" s="123"/>
+      <c r="L80" s="123"/>
+      <c r="M80" s="123"/>
+      <c r="N80" s="123"/>
+    </row>
+    <row r="82" spans="9:14">
+      <c r="I82" s="123"/>
+      <c r="J82" s="123"/>
+      <c r="K82" s="123"/>
+      <c r="L82" s="123"/>
+      <c r="M82" s="123"/>
+      <c r="N82" s="123"/>
+    </row>
+    <row r="88" spans="9:14">
+      <c r="I88" s="82"/>
+      <c r="J88" s="82"/>
+      <c r="K88" s="82"/>
+      <c r="L88" s="82"/>
+      <c r="M88" s="82"/>
+      <c r="N88" s="82"/>
+    </row>
+    <row r="89" spans="9:14">
+      <c r="I89" s="82"/>
+      <c r="J89" s="82"/>
+      <c r="K89" s="82"/>
+      <c r="L89" s="82"/>
+      <c r="M89" s="82"/>
+      <c r="N89" s="82"/>
+    </row>
+    <row r="90" spans="9:14">
+      <c r="I90" s="82"/>
+      <c r="J90" s="82"/>
+      <c r="K90" s="82"/>
+      <c r="L90" s="82"/>
+      <c r="M90" s="82"/>
+      <c r="N90" s="82"/>
+    </row>
+    <row r="91" spans="9:14">
+      <c r="I91" s="82"/>
+      <c r="J91" s="82"/>
+      <c r="K91" s="82"/>
+      <c r="L91" s="82"/>
+      <c r="M91" s="82"/>
+      <c r="N91" s="82"/>
+    </row>
+    <row r="92" spans="9:14">
+      <c r="I92" s="82"/>
+      <c r="J92" s="82"/>
+      <c r="K92" s="82"/>
+      <c r="L92" s="82"/>
+      <c r="M92" s="82"/>
+      <c r="N92" s="82"/>
+    </row>
+    <row r="93" spans="9:14">
+      <c r="I93" s="82"/>
+      <c r="J93" s="82"/>
+      <c r="K93" s="82"/>
+      <c r="L93" s="82"/>
+      <c r="M93" s="82"/>
+      <c r="N93" s="82"/>
+    </row>
+    <row r="94" spans="9:14">
+      <c r="I94" s="82"/>
+      <c r="J94" s="82"/>
+      <c r="K94" s="82"/>
+      <c r="L94" s="82"/>
+      <c r="M94" s="82"/>
+      <c r="N94" s="82"/>
+    </row>
+    <row r="95" spans="9:14">
+      <c r="I95" s="82"/>
+      <c r="J95" s="82"/>
+      <c r="K95" s="82"/>
+      <c r="L95" s="82"/>
+      <c r="M95" s="82"/>
+      <c r="N95" s="82"/>
+    </row>
+    <row r="96" spans="9:14">
+      <c r="I96" s="82"/>
+      <c r="J96" s="82"/>
+      <c r="K96" s="82"/>
+      <c r="L96" s="82"/>
+      <c r="M96" s="82"/>
+      <c r="N96" s="82"/>
+    </row>
+    <row r="97" spans="9:14">
+      <c r="I97" s="82"/>
+      <c r="J97" s="82"/>
+      <c r="K97" s="82"/>
+      <c r="L97" s="82"/>
+      <c r="M97" s="82"/>
+      <c r="N97" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="39">
+    <mergeCell ref="N44:N45"/>
+    <mergeCell ref="O44:O45"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="U44:U45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="M44:M45"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+  </mergeCells>
+  <phoneticPr fontId="2"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N46:N49" xr:uid="{78DF3EDD-C15B-944E-A662-07EE3A4C5079}">
+      <formula1>qeryKind</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O46:O49" xr:uid="{C4FC505B-E3FB-8042-A4BE-8C4F7BCCCDCF}">
+      <formula1>isNullable</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17 C19:C20" xr:uid="{FB74024D-2E65-4447-9843-D6FCFAB97D07}">
+      <formula1>isImport</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{1F3BD804-9FF4-CE43-84DC-80E4653AE15A}">
+      <formula1>Validate実装パターン</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D&amp;  &amp;T</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C9CEA9-BB18-7040-B693-BE70092DD3E6}">
+          <x14:formula1>
+            <xm:f>config!$B$5:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G46:G49</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{98D03428-FFFA-CC48-A00C-87C0ADD14FDB}">
+          <x14:formula1>
+            <xm:f>config!$D$5:$D$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{3CF8A77B-F4D5-CB41-B0E4-018862C374CA}">
+          <x14:formula1>
+            <xm:f>config!$D$5:$D$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C10:C12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{62881BDE-759B-C443-85B5-994A2C8C56AF}">
+          <x14:formula1>
+            <xm:f>config!$C$5:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE71A976-2A0D-FC48-8407-D1D2B098B2FF}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T65"/>
+  <sheetViews>
+    <sheetView zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="20.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="43.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="6.1640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.1640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="18.83203125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.33203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="9.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.83203125" style="1"/>
+    <col min="31" max="31" width="9.1640625" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="19">
+      <c r="A1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="106" t="str">
+        <f>process!D6&amp;PROPER(C9)&amp;IF(C8="要求電文(C→S)", "Request", "Response")</f>
+        <v>SampleArrayPayloadTestPutResponse</v>
+      </c>
+      <c r="D6" s="105"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="Q7"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" s="72"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="146" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="146"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="146" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="146"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="98" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="98"/>
+      <c r="C12" s="136" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="136"/>
+      <c r="E12" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="98"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="99" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="100"/>
+      <c r="C14" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="99" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="100"/>
+      <c r="C15" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="6"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="178" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="178"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="178"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="178"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="172" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="173"/>
+      <c r="D18" s="173"/>
+      <c r="E18" s="173"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="82"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="S18" s="88"/>
+      <c r="T18" s="88"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="93"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="155"/>
+      <c r="G19" s="155"/>
+      <c r="H19" s="89"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="N19" s="89"/>
+      <c r="O19" s="89"/>
+      <c r="P19" s="89"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="94"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="156"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="89"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="89"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="95"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
+      <c r="H21" s="89"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="89"/>
+      <c r="P21" s="89"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="C22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22" s="89"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="175" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="176"/>
+      <c r="C23" s="176"/>
+      <c r="D23" s="176"/>
+      <c r="E23" s="176"/>
+      <c r="F23" s="176"/>
+      <c r="G23" s="177"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23" s="89"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="161" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="161"/>
+      <c r="D24" s="161"/>
+      <c r="E24" s="161"/>
+      <c r="F24" s="161"/>
+      <c r="G24" s="161"/>
+      <c r="H24" s="82"/>
+      <c r="M24" s="89"/>
+      <c r="N24" s="82"/>
+      <c r="O24" s="82"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="82"/>
+      <c r="S24" s="88"/>
+      <c r="T24" s="88"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="93">
+        <v>1</v>
+      </c>
+      <c r="B25" s="162" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="162"/>
+      <c r="D25" s="162"/>
+      <c r="E25" s="162"/>
+      <c r="F25" s="162"/>
+      <c r="G25" s="162"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="89"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="93">
+        <v>2</v>
+      </c>
+      <c r="B26" s="162" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" s="162"/>
+      <c r="D26" s="162"/>
+      <c r="E26" s="162"/>
+      <c r="F26" s="162"/>
+      <c r="G26" s="162"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="N26" s="89"/>
+      <c r="O26" s="89"/>
+      <c r="P26" s="89"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="94">
+        <v>3</v>
+      </c>
+      <c r="B27" s="163" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="163"/>
+      <c r="D27" s="163"/>
+      <c r="E27" s="163"/>
+      <c r="F27" s="163"/>
+      <c r="G27" s="163"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="89"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="93">
+        <v>4</v>
+      </c>
+      <c r="B28" s="162" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="162"/>
+      <c r="D28" s="162"/>
+      <c r="E28" s="162"/>
+      <c r="F28" s="162"/>
+      <c r="G28" s="162"/>
+      <c r="H28" s="89"/>
+      <c r="M28" s="89"/>
+      <c r="N28" s="89"/>
+      <c r="O28" s="89"/>
+      <c r="P28" s="89"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="94"/>
+      <c r="B29" s="162"/>
+      <c r="C29" s="162"/>
+      <c r="D29" s="162"/>
+      <c r="E29" s="162"/>
+      <c r="F29" s="162"/>
+      <c r="G29" s="162"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="89"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="95"/>
+      <c r="B30" s="164"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="89"/>
+      <c r="O30" s="89"/>
+      <c r="P30" s="89"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31" s="89"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="175" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="176"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="176"/>
+      <c r="F32" s="176"/>
+      <c r="G32" s="177"/>
+      <c r="M32" s="89"/>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="161" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="161"/>
+      <c r="D33" s="161"/>
+      <c r="E33" s="161"/>
+      <c r="F33" s="161"/>
+      <c r="G33" s="161"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
+      <c r="S33" s="88"/>
+      <c r="T33" s="88"/>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="93"/>
+      <c r="B34" s="155"/>
+      <c r="C34" s="155"/>
+      <c r="D34" s="155"/>
+      <c r="E34" s="155"/>
+      <c r="F34" s="155"/>
+      <c r="G34" s="185"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="89"/>
+      <c r="P34" s="89"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="94"/>
+      <c r="B35" s="156"/>
+      <c r="C35" s="156"/>
+      <c r="D35" s="156"/>
+      <c r="E35" s="156"/>
+      <c r="F35" s="156"/>
+      <c r="G35" s="186"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="89"/>
+      <c r="P35" s="89"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="95"/>
+      <c r="B36" s="157"/>
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="187"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37" s="89"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="6"/>
+      <c r="M38" s="89"/>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="119"/>
+      <c r="L39" s="119"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="45"/>
+    </row>
+    <row r="40" spans="1:20" ht="15">
+      <c r="A40" s="191" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="191" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="191" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="191" t="s">
+        <v>129</v>
+      </c>
+      <c r="F40" s="191" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="191" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="191" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40" s="204" t="s">
+        <v>168</v>
+      </c>
+      <c r="J40" s="206" t="s">
+        <v>169</v>
+      </c>
+      <c r="K40" s="206" t="s">
+        <v>170</v>
+      </c>
+      <c r="L40" s="197" t="s">
+        <v>171</v>
+      </c>
+      <c r="M40" s="188" t="s">
+        <v>148</v>
+      </c>
+      <c r="N40" s="201" t="s">
+        <v>99</v>
+      </c>
+      <c r="O40" s="202"/>
+      <c r="P40" s="203" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q40" s="202"/>
+      <c r="R40" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="S40" s="191" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15">
+      <c r="A41" s="200"/>
+      <c r="B41" s="200"/>
+      <c r="C41" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="200"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="200"/>
+      <c r="H41" s="200"/>
+      <c r="I41" s="205"/>
+      <c r="J41" s="207"/>
+      <c r="K41" s="207"/>
+      <c r="L41" s="208"/>
+      <c r="M41" s="199"/>
+      <c r="N41" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="O41" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="P41" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q41" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="R41" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="S41" s="200"/>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="A42" s="51">
+        <v>1</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="120"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="128"/>
+      <c r="L42" s="120"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="54"/>
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="54"/>
+      <c r="S42" s="55"/>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="A43" s="51">
+        <f>A42+1</f>
+        <v>2</v>
+      </c>
+      <c r="B43" s="112" t="s">
+        <v>206</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="113" t="s">
+        <v>208</v>
+      </c>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="121"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="122"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="114"/>
+      <c r="N43" s="54"/>
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="54"/>
+      <c r="S43" s="55"/>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="A44" s="51"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="121"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="54"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="52"/>
+      <c r="P44" s="52"/>
+      <c r="Q44" s="52"/>
+      <c r="R44" s="52"/>
+      <c r="S44" s="55"/>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" s="51"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="121"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="129"/>
+      <c r="L45" s="121"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="52"/>
+      <c r="P45" s="52"/>
+      <c r="Q45" s="52"/>
+      <c r="R45" s="52"/>
+      <c r="S45" s="58"/>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="A46" s="51"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="117"/>
+      <c r="H46" s="116"/>
+      <c r="I46" s="122"/>
+      <c r="J46" s="122"/>
+      <c r="K46" s="129"/>
+      <c r="L46" s="122"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="52"/>
+      <c r="P46" s="52"/>
+      <c r="Q46" s="52"/>
+      <c r="R46" s="52"/>
+      <c r="S46" s="58"/>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="59"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="124"/>
+      <c r="J47" s="125"/>
+      <c r="K47" s="125"/>
+      <c r="L47" s="126"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="63"/>
+      <c r="R47" s="63"/>
+      <c r="S47" s="64"/>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="I48" s="123"/>
+      <c r="J48" s="123"/>
+      <c r="K48" s="123"/>
+      <c r="L48" s="123"/>
+    </row>
+    <row r="50" spans="9:12">
+      <c r="I50" s="123"/>
+      <c r="J50" s="123"/>
+      <c r="K50" s="123"/>
+      <c r="L50" s="123"/>
+    </row>
+    <row r="56" spans="9:12">
+      <c r="I56" s="82"/>
+      <c r="J56" s="82"/>
+      <c r="K56" s="82"/>
+      <c r="L56" s="82"/>
+    </row>
+    <row r="57" spans="9:12">
+      <c r="I57" s="82"/>
+      <c r="J57" s="82"/>
+      <c r="K57" s="82"/>
+      <c r="L57" s="82"/>
+    </row>
+    <row r="58" spans="9:12">
+      <c r="I58" s="82"/>
+      <c r="J58" s="82"/>
+      <c r="K58" s="82"/>
+      <c r="L58" s="82"/>
+    </row>
+    <row r="59" spans="9:12">
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="82"/>
+    </row>
+    <row r="60" spans="9:12">
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+    </row>
+    <row r="61" spans="9:12">
+      <c r="I61" s="82"/>
+      <c r="J61" s="82"/>
+      <c r="K61" s="82"/>
+      <c r="L61" s="82"/>
+    </row>
+    <row r="62" spans="9:12">
+      <c r="I62" s="82"/>
+      <c r="J62" s="82"/>
+      <c r="K62" s="82"/>
+      <c r="L62" s="82"/>
+    </row>
+    <row r="63" spans="9:12">
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="82"/>
+      <c r="L63" s="82"/>
+    </row>
+    <row r="64" spans="9:12">
+      <c r="I64" s="82"/>
+      <c r="J64" s="82"/>
+      <c r="K64" s="82"/>
+      <c r="L64" s="82"/>
+    </row>
+    <row r="65" spans="9:12">
+      <c r="I65" s="82"/>
+      <c r="J65" s="82"/>
+      <c r="K65" s="82"/>
+      <c r="L65" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="S40:S41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:G18"/>
+  </mergeCells>
+  <phoneticPr fontId="2"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M42:M47" xr:uid="{9043EFF1-5C4B-B949-B6EA-FD8F4F349A22}">
+      <formula1>isNullable</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C15" xr:uid="{13D337BD-E6A4-9A46-BD5C-CAEC05CEB1E0}">
+      <formula1>isImport</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{B6B2DEBC-D063-AF48-ACAC-293D9BDEF841}">
+      <formula1>Validate実装パターン</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D&amp;  &amp;T</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{73E701E3-C149-7F49-BAED-668AC18753C9}">
+          <x14:formula1>
+            <xm:f>config!$B$5:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G42:G47</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{ECE96ABC-84D6-9C4C-9163-8E47B36FAA3E}">
+          <x14:formula1>
+            <xm:f>config!$C$5:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -9993,7 +12340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -10051,13 +12398,13 @@
         <v>149</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -10081,10 +12428,10 @@
         <v>111</v>
       </c>
       <c r="H5" s="131" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I5" s="38" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -10102,10 +12449,10 @@
       <c r="F6" s="53"/>
       <c r="G6" s="53"/>
       <c r="H6" s="132" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -10118,7 +12465,7 @@
       </c>
       <c r="H7" s="133"/>
       <c r="I7" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:9">

</xml_diff>